<commit_message>
aktualizacja bledow i ulepszen
</commit_message>
<xml_diff>
--- a/Apteka Słonik - błędy i ulepszenia.xlsx
+++ b/Apteka Słonik - błędy i ulepszenia.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Paulina1\Documents\Paulina\cherry IT kurs\Portfolio\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C58E3DE8-883B-41F3-92E8-47E0108EFC0E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4AF6E66-D695-4A66-9754-5CF8CC88F54B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9060" xr2:uid="{9801ED63-41E7-4471-A66C-D3BB2A2C2D26}"/>
   </bookViews>
@@ -68,10 +68,6 @@
     <t>Podczas powiększania strony np.. Do 125% lub 175% przycisk "KONTAKT" z panelu głównego przemieszcza się pod ten panel.</t>
   </si>
   <si>
-    <t>1. Otwórz przeglądarkę i przejdź na stronę http://www.aptekaslonik.pl/.
-2. Ustaw powiększenie przeglądarki na 100%, a następnie na 125% i zaobserwój co się dzieje z przyciskiem "KONTAKT" z panelu głównego.</t>
-  </si>
-  <si>
     <t>High</t>
   </si>
   <si>
@@ -102,9 +98,6 @@
     <t>Strona główna - przycisk KONTAKT przemieszcza się poniżej głównego panelu podczas powiększenia okna przeglądarki.</t>
   </si>
   <si>
-    <t xml:space="preserve">Strona główna - przyciski "SZUKAJ", "ZAPISZ" i "WYPISZ" są za blisko okna pod którym się znajdują - brak dostępu. </t>
-  </si>
-  <si>
     <t>Strona główna - słaba jakość grafiki banerów, przycisków i zdjęć produktów podczas powiększenia strony.</t>
   </si>
   <si>
@@ -112,10 +105,6 @@
   </si>
   <si>
     <t xml:space="preserve">Tabele na stronie powinny być jednakowej szerokości - wygląda to bardziej estetycznie. </t>
-  </si>
-  <si>
-    <t xml:space="preserve">1. Otwórz przeglądarkę i przejdź na stronę http://www.aptekaslonik.pl/.
-2. Przyjrzyj się szerokości wszystkich tabel znajdujących się na stronie </t>
   </si>
   <si>
     <t>Strona główna - tabele "KOSMETYKI PRODUCENT", "NOWOŚCI" i "FARMACEUTA POLECA RÓWNIEŻ" są szersze od tabel powyżej.</t>
@@ -128,13 +117,6 @@
     <t xml:space="preserve">Strona główna - nieujednolicony sposób przekierowania na inną stronę  przez banery i przyciski. </t>
   </si>
   <si>
-    <t xml:space="preserve">Niektóre banery/przyciski kierują na inną stronę otwierająć ją w tej samej karcie przeglądarki, niektóre w nowej karcie, a niektóre przyciski nie działają. </t>
-  </si>
-  <si>
-    <t>1. Otwórz przeglądarkę i przejdź na stronę http://www.aptekaslonik.pl/.
-2. Klikaj po kolei we wszystkie banery i przyciski znajdujące się na stronie głównej w jej środkowej części (bez bocznych paneli) i zwróć uwagę, czy otwierają nowe strony w aktualnej czy nowej karcie przeglądarki. Większość stron otwiera się w aktualnej karcie pzreglądarki, w nowej karcie pzreglądarki otwierają strony banery/przyciski: "UBEZPIECZENIE", "NOWOŚĆ", "PROMOCJA" i "POLECAMY". Nie działają banery: "ZWROT", "GWARANACJA".</t>
-  </si>
-  <si>
     <t>Strona główna - brak odstępu pomiędzy tabelami "KOSMETYKI PRODUCENT" i "NOWOŚCI".</t>
   </si>
   <si>
@@ -143,9 +125,6 @@
   </si>
   <si>
     <t>Strona główna - puste komórki w tabelach.</t>
-  </si>
-  <si>
-    <t>W dwóch tabelach widoczne są niepotzrebne puste komórki.</t>
   </si>
   <si>
     <t>1. Otwórz przeglądarkę i przejdź na stronę http://www.aptekaslonik.pl/.
@@ -160,15 +139,6 @@
     <t>Strona główna - niejednolite wyśrodkowanie tekstu w tabeli.</t>
   </si>
   <si>
-    <t>1. Otwórz przeglądarkę i przejdź na stronę http://www.aptekaslonik.pl/.
-2. Zjedź w dół strony do tabeli "KOSMETYKI I PRODUKTY POLECANE". Pod nagłówkiem w koeljnym wierszu teksty w obu kolumnach nie są jednakowo wyśrodkowane.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Marka Vichy powinna być poprzedzona takim samym znacznikiem jak reszta marek w tabeli. 
-Przecinek po ostatnim wymienionym produkcie jest zbędny.
-Po ostatniej linijce tekstu w tabeli powinien być niewielki odstęp, tak aby litery nie nachodizły na obramowanie tabeli. </t>
-  </si>
-  <si>
     <t xml:space="preserve">1. Otwórz przeglądarkę i przejdź na stronę http://www.aptekaslonik.pl/.
 2. Zjedź w dół strony do tabeli "KOSMETYKI PRODUCENT". </t>
   </si>
@@ -179,12 +149,6 @@
     <t>1. Otwórz przeglądarkę i przejdź na stronę http://www.aptekaslonik.pl/.
 2. Z głównego panelu wybierz "O APTECE". 
 3. Zjedź do logo i zdjęcia apteki.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Bezpieczeństwo, Regulamin, Dostawa - brak wyjustowania tesktu do obu stron. </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Tekst jest wyjustowany do lewej strony - bardzej profesjonalnie wyglądał by wyjustowany do obu stron. </t>
   </si>
   <si>
     <t xml:space="preserve">1. Otwórz przeglądarkę i przejdź na stronę http://www.aptekaslonik.pl/.
@@ -210,20 +174,7 @@
 </t>
   </si>
   <si>
-    <t xml:space="preserve">1. Otwórz przeglądarkę i przejdź na stronę http://www.aptekaslonik.pl/.
-2.  Z głównego panelu wybierz "POMOC". Przyhrzyj się screenom zawartym w tabeli - są bardzo słabej jakości
-</t>
-  </si>
-  <si>
     <t>Wyszukiwanie zaawansowane - nie działa opcja wyszukiwania "od" konkretnej ceny.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1. Otwórz przeglądarkę i przejdź na stronę http://www.aptekaslonik.pl/.
-2.  Z lewej strony widoczna jest wyszukiwarka. Kliknij w napis "WYSZUKIWANIE ZAAWANSOWANE" - otworzy się strona umożliwiająca wyszukiwanie wg kryteriów.
-3. W pole wyszukiwania wpisz "krem" i kliknij przycisk "SZUKAJ".
-4. Pojawi się lista wyników. Klikniij na nagłówek "DAWKA" - pojawi się biały trójkąt, który powinien być skierowany kiedy lista produktów jest sortowana rosnąco, a w dół - gdy jest sortowana malejąco wg dawki. 
-5. Kilkukrotnie klikniej w nagłówek "DAWKA" i obserwuj jak sortowane są wyniki - wyniki nie są sortowane wg DAWKI. 
-</t>
   </si>
   <si>
     <t>FAQ - nieprawidłowy drugi cudzysłów przy słowie "POMOC".</t>
@@ -260,15 +211,6 @@
 </t>
   </si>
   <si>
-    <t xml:space="preserve">1. Otwórz przeglądarkę i przejdź na stronę http://www.aptekaslonik.pl/.
-2.  Z lewej strony widoczna jest wyszukiwarka. Kliknij w napis "WYSZUKIWANIE ZAAWANSOWANE" - otworzy się strona umożliwiająca wyszukiwanie wg kryteriów.
-3. W pole wyszukiwania wpisz "tonik". Zobacz, że nie ma możliwości zaznaczenia, aby w wynikach pojawiły się tylko produkty dostępne. 
-4. Kliknij przycisk "SZUKAJ".
-5. Pojawi się lista wyników. Przejrzyj strony z wynikami i znajdź wynik z napisem "Zapytaj o dostępność". 
-7. Wybierz jeden taki produkt i do niego przejdź. Spróboj kliknąć w komunikat "Zapytaj o dostępność" - nic się nie dzieje.
-</t>
-  </si>
-  <si>
     <t xml:space="preserve">Rejestracja - brak walidacji pół w formularzu  - można wpisać cokolwiek. </t>
   </si>
   <si>
@@ -371,35 +313,12 @@
     <t>21.02.2019</t>
   </si>
   <si>
-    <t xml:space="preserve">Zapytaj farmaceutę - brak polskich liter w komunikacie podczas próby wysłania pustego zapytania. </t>
-  </si>
-  <si>
     <t>Database error i MySQL Error podczas przeglądania produktów znajdujących się na podstronach z wynikami między 10 a 20 i próbie wrócenia do 10 strony z wynikami za pomocą przycisku "&lt;&lt;".</t>
   </si>
   <si>
-    <t>1. Otwórz przeglądarkę i przejdź na stronę http://www.aptekaslonik.pl/.
-2.  Z prawej strony widać zakładkę Zapytaj farmaceutę. Kliknij poniżej w "Zapytaj farmaceutę".
-3. Nie wpisuj nic w formularz tylko kliknij "Zadaj pytanie". Pojawia się komunikat ze znakiem zapytania zamiast polskiego znaku: "Wymangane jest pole Imi  i nazwisko
-Wymangane jest pole adres e-mail
-Wymangane jest pole pytanie".</t>
-  </si>
-  <si>
-    <t>komunikat ze znakiem zapytania zamiast polskiego znaku: "Wymangane jest pole Imi� i nazwisko
-Wymangane jest pole adres e-mail
-Wymangane jest pole pytanie".</t>
-  </si>
-  <si>
     <t>Strona główna - baner Avene znajdujący się z prawej strony przeglądarki nie działa.</t>
   </si>
   <si>
-    <t xml:space="preserve">1. Otwórz przeglądarkę i przejdź na stronę http://www.aptekaslonik.pl/.
-2.  Z prawej strony, pod napisem "Apteka kosmetyki" widać banery różnych marek. Znajdź banere "Avene" i kliknij w niego. Nic się nie dzieje, nie przekierowuje do tabeli z wymienionymi kategoriami produktów marki Avene.
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Strona główna - tabela "KOSMETYKI PRODUCENT" - brak znacznika przed marką Vichy, niepotrzebny przecinek po ostanim słowie w tabeli, brak odstępu po ostatniej linijce tekstu. </t>
-  </si>
-  <si>
     <t xml:space="preserve">O aptece - słabej jakości logo i zdjęcie apteki. </t>
   </si>
   <si>
@@ -410,9 +329,6 @@
   </si>
   <si>
     <t>Produkcyjne</t>
-  </si>
-  <si>
-    <t>Strona główna - baner "Zapytaj farmaceutę" rozjeżdzą się podczas powiększenia strony do 150% i wychodzi poza obramowanie.</t>
   </si>
   <si>
     <t>Strona główna - tabele "NOWOŚCI" i "FARMACEUTA POLECA RÓWNIEŻ" - widać, że panel nagłówkowy tabel jest złączony z dwóch i wygląda nieestetycznie.</t>
@@ -436,6 +352,90 @@
   </si>
   <si>
     <t>Sło-026</t>
+  </si>
+  <si>
+    <t>1. Otwórz przeglądarkę i przejdź na stronę http://www.aptekaslonik.pl/.
+2. Ustaw powiększenie przeglądarki na 100%, a następnie na 125% i zaobserwuj co się dzieje z przyciskiem "KONTAKT" z panelu głównego.</t>
+  </si>
+  <si>
+    <t>Strona główna - baner "Zapytaj farmaceutę" rozjeżdżają się podczas powiększenia strony do 150% i wychodzi poza obramowanie.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Niektóre banery/przyciski kierują na inną stronę otwierając ją w tej samej karcie przeglądarki, niektóre w nowej karcie, a niektóre przyciski nie działają. </t>
+  </si>
+  <si>
+    <t>1. Otwórz przeglądarkę i przejdź na stronę http://www.aptekaslonik.pl/.
+2. Klikaj po kolei we wszystkie banery i przyciski znajdujące się na stronie głównej w jej środkowej części (bez bocznych paneli) i zwróć uwagę, czy otwierają nowe strony w aktualnej czy nowej karcie przeglądarki. Większość stron otwiera się w aktualnej karcie przeglądarki, w nowej karcie przeglądarki otwierają strony banery/przyciski: "UBEZPIECZENIE", "NOWOŚĆ", "PROMOCJA" i "POLECAMY". Nie działają banery: "ZWROT", "GWARANCJA".</t>
+  </si>
+  <si>
+    <t>W dwóch tabelach widoczne są niepotrzebne puste komórki.</t>
+  </si>
+  <si>
+    <t>1. Otwórz przeglądarkę i przejdź na stronę http://www.aptekaslonik.pl/.
+2. Zjedź w dół strony do tabeli "KOSMETYKI I PRODUKTY POLECANE". Pod nagłówkiem w kolejnym wierszu teksty w obu kolumnach nie są jednakowo wyśrodkowane.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Strona główna - tabela "KOSMETYKI PRODUCENT" - brak znacznika przed marką Vichy, niepotrzebny przecinek po ostatnim słowie w tabeli, brak odstępu po ostatniej linijce tekstu. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Marka Vichy powinna być poprzedzona takim samym znacznikiem jak reszta marek w tabeli. 
+Przecinek po ostatnim wymienionym produkcie jest zbędny.
+Po ostatniej linijce tekstu w tabeli powinien być niewielki odstęp, tak aby litery nie nachodziły na obramowanie tabeli. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Otwórz przeglądarkę i przejdź na stronę http://www.aptekaslonik.pl/.
+2.  Z lewej strony widoczna jest wyszukiwarka. Kliknij w napis "WYSZUKIWANIE ZAAWANSOWANE" - otworzy się strona umożliwiająca wyszukiwanie wg kryteriów.
+3. W pole wyszukiwania wpisz "krem" i kliknij przycisk "SZUKAJ".
+4. Pojawi się lista wyników. Kliknij na nagłówek "DAWKA" - pojawi się biały trójkąt, który powinien być skierowany kiedy lista produktów jest sortowana rosnąco, a w dół - gdy jest sortowana malejąco wg dawki. 
+5. Kilkukrotnie kliknij w nagłówek "DAWKA" i obserwuj jak sortowane są wyniki - wyniki nie są sortowane wg DAWKI. 
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Otwórz przeglądarkę i przejdź na stronę http://www.aptekaslonik.pl/.
+2.  Z lewej strony widoczna jest wyszukiwarka. Kliknij w napis "WYSZUKIWANIE ZAAWANSOWANE" - otworzy się strona umożliwiająca wyszukiwanie wg kryteriów.
+3. W pole wyszukiwania wpisz "tonik". Zobacz, że nie ma możliwości zaznaczenia, aby w wynikach pojawiły się tylko produkty dostępne. 
+4. Kliknij przycisk "SZUKAJ".
+5. Pojawi się lista wyników. Przejrzyj strony z wynikami i znajdź wynik z napisem "Zapytaj o dostępność". 
+7. Wybierz jeden taki produkt i do niego przejdź. Spróbuj kliknąć w komunikat "Zapytaj o dostępność" - nic się nie dzieje.
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Zapytaj farmaceutę - brak polskich liter i literówka w komunikacie podczas próby wysłania pustego zapytania. </t>
+  </si>
+  <si>
+    <t>Komunikat ze znakiem zapytania zamiast polskiego znaku oraz literówką w słowie "wymagane": "Wymangane jest pole Imi� i nazwisko
+Wymangane jest pole adres e-mail
+Wymangane jest pole pytanie".</t>
+  </si>
+  <si>
+    <t>1. Otwórz przeglądarkę i przejdź na stronę http://www.aptekaslonik.pl/.
+2.  Z prawej strony widać zakładkę Zapytaj farmaceutę. Kliknij poniżej w "Zapytaj farmaceutę".
+3. Nie wpisuj nic w formularz tylko kliknij "Zadaj pytanie". Pojawia się komunikat ze znakiem zapytania zamiast polskiego znaku i literówką: "Wymangane jest pole Imi  i nazwisko
+Wymangane jest pole adres e-mail
+Wymangane jest pole pytanie".</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Otwórz przeglądarkę i przejdź na stronę http://www.aptekaslonik.pl/.
+2.  Z prawej strony, pod napisem "Apteka kosmetyki" widać banery różnych marek. Znajdź baner "Avene" i kliknij w niego. Nic się nie dzieje, nie przekierowuje do tabeli z wymienionymi kategoriami produktów marki Avene.
+</t>
+  </si>
+  <si>
+    <t>1. Otwórz przeglądarkę i przejdź na stronę http://www.aptekaslonik.pl/.
+2. Przyjrzyj się szerokości wszystkich tabel znajdujących się na stronie.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bezpieczeństwo, Regulamin, Dostawa - brak wyjustowania tekstu do obu stron. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tekst jest wyjustowany do lewej strony - bardziej profesjonalnie wyglądał by wyjustowany do obu stron. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Otwórz przeglądarkę i przejdź na stronę http://www.aptekaslonik.pl/.
+2.  Z głównego panelu wybierz "POMOC". Przyjrzyj się screenom zawartym w tabeli - są bardzo słabej jakości
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Strona główna - przyciski "SZUKAJ", "ZAPISZ" i "WYPISZ" są za blisko okna pod którym się znajdują - brak odstępu. </t>
   </si>
 </sst>
 </file>
@@ -1305,7 +1305,7 @@
       <xdr:col>11</xdr:col>
       <xdr:colOff>3930713</xdr:colOff>
       <xdr:row>28</xdr:row>
-      <xdr:rowOff>3354</xdr:rowOff>
+      <xdr:rowOff>3355</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1860,8 +1860,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4AB430F7-4116-4B45-93F7-26D381EF7FF2}">
   <dimension ref="C2:M53"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="82" zoomScaleNormal="82" workbookViewId="0">
-      <selection activeCell="C27" sqref="C27:C35"/>
+    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="82" zoomScaleNormal="82" workbookViewId="0">
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1880,7 +1880,7 @@
   <sheetData>
     <row r="2" spans="3:13" ht="25.8" x14ac:dyDescent="0.5">
       <c r="C2" s="16" t="s">
-        <v>107</v>
+        <v>88</v>
       </c>
       <c r="D2" s="17"/>
       <c r="E2" s="17"/>
@@ -1913,7 +1913,7 @@
         <v>5</v>
       </c>
       <c r="I4" s="2" t="s">
-        <v>55</v>
+        <v>43</v>
       </c>
       <c r="J4" s="1" t="s">
         <v>6</v>
@@ -1927,28 +1927,28 @@
     </row>
     <row r="5" spans="3:13" ht="352.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C5" s="3" t="s">
-        <v>65</v>
+        <v>52</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E5" s="3" t="s">
         <v>11</v>
       </c>
       <c r="F5" s="7" t="s">
-        <v>12</v>
+        <v>92</v>
       </c>
       <c r="G5" s="4" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="H5" s="13" t="s">
-        <v>103</v>
+        <v>85</v>
       </c>
       <c r="I5" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="J5" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="K5" s="3" t="s">
         <v>10</v>
@@ -1957,26 +1957,26 @@
     </row>
     <row r="6" spans="3:13" ht="249.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C6" s="3" t="s">
-        <v>66</v>
+        <v>53</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>104</v>
+        <v>93</v>
       </c>
       <c r="E6" s="5"/>
       <c r="F6" s="7" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G6" s="5" t="s">
         <v>9</v>
       </c>
       <c r="H6" s="8" t="s">
-        <v>103</v>
+        <v>85</v>
       </c>
       <c r="I6" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="J6" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="K6" s="5" t="s">
         <v>10</v>
@@ -1986,28 +1986,28 @@
     </row>
     <row r="7" spans="3:13" ht="240.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C7" s="3" t="s">
-        <v>67</v>
+        <v>54</v>
       </c>
       <c r="D7" s="5" t="s">
+        <v>110</v>
+      </c>
+      <c r="E7" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="F7" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="G7" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="E7" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="F7" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="G7" s="5" t="s">
-        <v>24</v>
-      </c>
       <c r="H7" s="8" t="s">
-        <v>103</v>
+        <v>85</v>
       </c>
       <c r="I7" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="J7" s="5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="K7" s="5" t="s">
         <v>10</v>
@@ -2017,28 +2017,28 @@
     </row>
     <row r="8" spans="3:13" ht="215.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C8" s="3" t="s">
-        <v>68</v>
+        <v>55</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="E8" s="5" t="s">
-        <v>30</v>
+        <v>94</v>
       </c>
       <c r="F8" s="7" t="s">
-        <v>31</v>
+        <v>95</v>
       </c>
       <c r="G8" s="5" t="s">
         <v>9</v>
       </c>
       <c r="H8" s="8" t="s">
-        <v>103</v>
+        <v>85</v>
       </c>
       <c r="I8" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="J8" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="K8" s="5" t="s">
         <v>10</v>
@@ -2046,30 +2046,30 @@
       <c r="L8" s="5"/>
       <c r="M8" s="9"/>
     </row>
-    <row r="9" spans="3:13" ht="144" x14ac:dyDescent="0.3">
+    <row r="9" spans="3:13" ht="156.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C9" s="3" t="s">
-        <v>69</v>
+        <v>56</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="E9" s="5" t="s">
-        <v>35</v>
+        <v>96</v>
       </c>
       <c r="F9" s="7" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="G9" s="5" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="H9" s="8" t="s">
-        <v>103</v>
+        <v>85</v>
       </c>
       <c r="I9" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="J9" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="K9" s="5" t="s">
         <v>10</v>
@@ -2079,26 +2079,26 @@
     </row>
     <row r="10" spans="3:13" ht="182.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C10" s="3" t="s">
-        <v>70</v>
+        <v>57</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="E10" s="5"/>
       <c r="F10" s="7" t="s">
-        <v>39</v>
+        <v>97</v>
       </c>
       <c r="G10" s="5" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="H10" s="8" t="s">
-        <v>103</v>
+        <v>85</v>
       </c>
       <c r="I10" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="J10" s="5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="K10" s="5" t="s">
         <v>10</v>
@@ -2108,28 +2108,28 @@
     </row>
     <row r="11" spans="3:13" ht="255.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C11" s="3" t="s">
-        <v>71</v>
+        <v>58</v>
       </c>
       <c r="D11" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="E11" s="5" t="s">
         <v>99</v>
       </c>
-      <c r="E11" s="5" t="s">
-        <v>40</v>
-      </c>
       <c r="F11" s="7" t="s">
-        <v>41</v>
+        <v>33</v>
       </c>
       <c r="G11" s="5" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="H11" s="8" t="s">
-        <v>103</v>
+        <v>85</v>
       </c>
       <c r="I11" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="J11" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="K11" s="5" t="s">
         <v>10</v>
@@ -2139,26 +2139,26 @@
     </row>
     <row r="12" spans="3:13" ht="120" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C12" s="3" t="s">
-        <v>72</v>
+        <v>59</v>
       </c>
       <c r="D12" s="5" t="s">
-        <v>47</v>
+        <v>37</v>
       </c>
       <c r="E12" s="5"/>
       <c r="F12" s="7" t="s">
-        <v>48</v>
+        <v>38</v>
       </c>
       <c r="G12" s="5" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="H12" s="8" t="s">
-        <v>103</v>
+        <v>85</v>
       </c>
       <c r="I12" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="J12" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="K12" s="5" t="s">
         <v>10</v>
@@ -2168,26 +2168,26 @@
     </row>
     <row r="13" spans="3:13" ht="129.6" x14ac:dyDescent="0.3">
       <c r="C13" s="3" t="s">
-        <v>73</v>
+        <v>60</v>
       </c>
       <c r="D13" s="5" t="s">
-        <v>54</v>
+        <v>42</v>
       </c>
       <c r="E13" s="5"/>
       <c r="F13" s="7" t="s">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="G13" s="5" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="H13" s="8" t="s">
-        <v>103</v>
+        <v>85</v>
       </c>
       <c r="I13" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="J13" s="5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="K13" s="5" t="s">
         <v>10</v>
@@ -2197,28 +2197,28 @@
     </row>
     <row r="14" spans="3:13" ht="274.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C14" s="3" t="s">
-        <v>74</v>
+        <v>61</v>
       </c>
       <c r="D14" s="5" t="s">
-        <v>101</v>
+        <v>83</v>
       </c>
       <c r="E14" s="5" t="s">
-        <v>102</v>
+        <v>84</v>
       </c>
       <c r="F14" s="7" t="s">
-        <v>53</v>
+        <v>100</v>
       </c>
       <c r="G14" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="H14" s="8" t="s">
+        <v>85</v>
+      </c>
+      <c r="I14" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="J14" s="5" t="s">
         <v>13</v>
-      </c>
-      <c r="H14" s="8" t="s">
-        <v>103</v>
-      </c>
-      <c r="I14" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="J14" s="5" t="s">
-        <v>14</v>
       </c>
       <c r="K14" s="5" t="s">
         <v>10</v>
@@ -2228,26 +2228,26 @@
     </row>
     <row r="15" spans="3:13" ht="361.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C15" s="3" t="s">
-        <v>75</v>
+        <v>62</v>
       </c>
       <c r="D15" s="5" t="s">
-        <v>52</v>
+        <v>41</v>
       </c>
       <c r="E15" s="5"/>
       <c r="F15" s="7" t="s">
-        <v>59</v>
+        <v>47</v>
       </c>
       <c r="G15" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="H15" s="8" t="s">
+        <v>85</v>
+      </c>
+      <c r="I15" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="J15" s="3" t="s">
         <v>13</v>
-      </c>
-      <c r="H15" s="8" t="s">
-        <v>103</v>
-      </c>
-      <c r="I15" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="J15" s="3" t="s">
-        <v>14</v>
       </c>
       <c r="K15" s="5" t="s">
         <v>10</v>
@@ -2257,26 +2257,26 @@
     </row>
     <row r="16" spans="3:13" ht="270.60000000000002" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C16" s="3" t="s">
-        <v>76</v>
+        <v>63</v>
       </c>
       <c r="D16" s="5" t="s">
-        <v>58</v>
+        <v>46</v>
       </c>
       <c r="E16" s="5"/>
       <c r="F16" s="7" t="s">
-        <v>61</v>
+        <v>101</v>
       </c>
       <c r="G16" s="5" t="s">
         <v>9</v>
       </c>
       <c r="H16" s="8" t="s">
-        <v>103</v>
+        <v>85</v>
       </c>
       <c r="I16" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="J16" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="K16" s="5" t="s">
         <v>10</v>
@@ -2286,26 +2286,26 @@
     </row>
     <row r="17" spans="3:13" ht="302.39999999999998" x14ac:dyDescent="0.3">
       <c r="C17" s="3" t="s">
-        <v>77</v>
+        <v>64</v>
       </c>
       <c r="D17" s="12" t="s">
-        <v>62</v>
+        <v>49</v>
       </c>
       <c r="E17" s="12"/>
       <c r="F17" s="10" t="s">
-        <v>109</v>
+        <v>90</v>
       </c>
       <c r="G17" s="12" t="s">
-        <v>106</v>
+        <v>87</v>
       </c>
       <c r="H17" s="8" t="s">
-        <v>103</v>
+        <v>85</v>
       </c>
       <c r="I17" s="12" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="J17" s="12" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="K17" s="12" t="s">
         <v>10</v>
@@ -2315,26 +2315,26 @@
     </row>
     <row r="18" spans="3:13" ht="166.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C18" s="3" t="s">
-        <v>78</v>
+        <v>65</v>
       </c>
       <c r="D18" s="5" t="s">
-        <v>63</v>
+        <v>50</v>
       </c>
       <c r="E18" s="5"/>
       <c r="F18" s="10" t="s">
-        <v>64</v>
+        <v>51</v>
       </c>
       <c r="G18" s="5" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="H18" s="8" t="s">
-        <v>103</v>
+        <v>85</v>
       </c>
       <c r="I18" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="J18" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="K18" s="5" t="s">
         <v>10</v>
@@ -2344,28 +2344,28 @@
     </row>
     <row r="19" spans="3:13" ht="298.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C19" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="D19" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="E19" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="F19" s="10" t="s">
+        <v>78</v>
+      </c>
+      <c r="G19" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="H19" s="8" t="s">
+        <v>85</v>
+      </c>
+      <c r="I19" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="J19" s="5" t="s">
         <v>79</v>
-      </c>
-      <c r="D19" s="5" t="s">
-        <v>94</v>
-      </c>
-      <c r="E19" s="5" t="s">
-        <v>90</v>
-      </c>
-      <c r="F19" s="10" t="s">
-        <v>91</v>
-      </c>
-      <c r="G19" s="5" t="s">
-        <v>106</v>
-      </c>
-      <c r="H19" s="8" t="s">
-        <v>103</v>
-      </c>
-      <c r="I19" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="J19" s="5" t="s">
-        <v>92</v>
       </c>
       <c r="K19" s="5" t="s">
         <v>10</v>
@@ -2375,28 +2375,28 @@
     </row>
     <row r="20" spans="3:13" ht="206.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C20" s="3" t="s">
-        <v>80</v>
+        <v>67</v>
       </c>
       <c r="D20" s="5" t="s">
-        <v>93</v>
+        <v>102</v>
       </c>
       <c r="E20" s="5" t="s">
-        <v>96</v>
+        <v>103</v>
       </c>
       <c r="F20" s="10" t="s">
-        <v>95</v>
+        <v>104</v>
       </c>
       <c r="G20" s="5" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="H20" s="8" t="s">
-        <v>103</v>
+        <v>85</v>
       </c>
       <c r="I20" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="J20" s="5" t="s">
-        <v>92</v>
+        <v>79</v>
       </c>
       <c r="K20" s="5" t="s">
         <v>10</v>
@@ -2406,26 +2406,26 @@
     </row>
     <row r="21" spans="3:13" ht="119.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C21" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="D21" s="5" t="s">
         <v>81</v>
-      </c>
-      <c r="D21" s="5" t="s">
-        <v>97</v>
       </c>
       <c r="E21" s="5"/>
       <c r="F21" s="12" t="s">
-        <v>98</v>
+        <v>105</v>
       </c>
       <c r="G21" s="5" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="H21" s="8" t="s">
-        <v>103</v>
+        <v>85</v>
       </c>
       <c r="I21" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="J21" s="5" t="s">
-        <v>92</v>
+        <v>79</v>
       </c>
       <c r="K21" s="5" t="s">
         <v>10</v>
@@ -2461,7 +2461,7 @@
     </row>
     <row r="24" spans="3:13" ht="25.8" x14ac:dyDescent="0.3">
       <c r="C24" s="14" t="s">
-        <v>108</v>
+        <v>89</v>
       </c>
       <c r="D24" s="15"/>
       <c r="E24" s="15"/>
@@ -2507,7 +2507,7 @@
         <v>5</v>
       </c>
       <c r="I26" s="2" t="s">
-        <v>55</v>
+        <v>43</v>
       </c>
       <c r="J26" s="1" t="s">
         <v>6</v>
@@ -2522,28 +2522,28 @@
     </row>
     <row r="27" spans="3:13" ht="402.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C27" s="3" t="s">
-        <v>82</v>
+        <v>69</v>
       </c>
       <c r="D27" s="3" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="E27" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="F27" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="F27" s="3" t="s">
-        <v>17</v>
-      </c>
       <c r="G27" s="3" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="H27" s="3" t="s">
-        <v>103</v>
+        <v>85</v>
       </c>
       <c r="I27" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="J27" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="K27" s="3" t="s">
         <v>10</v>
@@ -2553,28 +2553,28 @@
     </row>
     <row r="28" spans="3:13" ht="306.60000000000002" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C28" s="5" t="s">
-        <v>83</v>
+        <v>70</v>
       </c>
       <c r="D28" s="5" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="E28" s="5" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="F28" s="5" t="s">
-        <v>26</v>
+        <v>106</v>
       </c>
       <c r="G28" s="5" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="H28" s="5" t="s">
-        <v>103</v>
+        <v>85</v>
       </c>
       <c r="I28" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="J28" s="5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="K28" s="5" t="s">
         <v>10</v>
@@ -2584,26 +2584,26 @@
     </row>
     <row r="29" spans="3:13" ht="213" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C29" s="3" t="s">
-        <v>84</v>
+        <v>71</v>
       </c>
       <c r="D29" s="5" t="s">
-        <v>105</v>
+        <v>86</v>
       </c>
       <c r="E29" s="5"/>
       <c r="F29" s="5" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="G29" s="5" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="H29" s="5" t="s">
-        <v>103</v>
+        <v>85</v>
       </c>
       <c r="I29" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="J29" s="5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="K29" s="5" t="s">
         <v>10</v>
@@ -2613,26 +2613,26 @@
     </row>
     <row r="30" spans="3:13" ht="308.39999999999998" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C30" s="5" t="s">
-        <v>85</v>
+        <v>72</v>
       </c>
       <c r="D30" s="5" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="E30" s="5"/>
       <c r="F30" s="5" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="G30" s="5" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="H30" s="5" t="s">
-        <v>103</v>
+        <v>85</v>
       </c>
       <c r="I30" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="J30" s="5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="K30" s="5" t="s">
         <v>10</v>
@@ -2642,26 +2642,26 @@
     </row>
     <row r="31" spans="3:13" ht="181.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C31" s="3" t="s">
-        <v>86</v>
+        <v>73</v>
       </c>
       <c r="D31" s="5" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="E31" s="5"/>
       <c r="F31" s="5" t="s">
-        <v>39</v>
+        <v>97</v>
       </c>
       <c r="G31" s="5" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="H31" s="5" t="s">
-        <v>103</v>
+        <v>85</v>
       </c>
       <c r="I31" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="J31" s="5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="K31" s="5" t="s">
         <v>10</v>
@@ -2671,28 +2671,28 @@
     </row>
     <row r="32" spans="3:13" ht="57.6" x14ac:dyDescent="0.3">
       <c r="C32" s="5" t="s">
-        <v>87</v>
+        <v>74</v>
       </c>
       <c r="D32" s="5" t="s">
-        <v>100</v>
+        <v>82</v>
       </c>
       <c r="E32" s="5" t="s">
-        <v>42</v>
+        <v>34</v>
       </c>
       <c r="F32" s="5" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
       <c r="G32" s="5" t="s">
         <v>9</v>
       </c>
       <c r="H32" s="5" t="s">
-        <v>103</v>
+        <v>85</v>
       </c>
       <c r="I32" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="J32" s="5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="K32" s="5" t="s">
         <v>10</v>
@@ -2702,28 +2702,28 @@
     </row>
     <row r="33" spans="3:13" ht="129.6" x14ac:dyDescent="0.3">
       <c r="C33" s="3" t="s">
-        <v>88</v>
+        <v>75</v>
       </c>
       <c r="D33" s="5" t="s">
-        <v>44</v>
+        <v>107</v>
       </c>
       <c r="E33" s="5" t="s">
-        <v>45</v>
+        <v>108</v>
       </c>
       <c r="F33" s="5" t="s">
-        <v>46</v>
+        <v>36</v>
       </c>
       <c r="G33" s="5" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="H33" s="5" t="s">
-        <v>103</v>
+        <v>85</v>
       </c>
       <c r="I33" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="J33" s="5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="K33" s="5" t="s">
         <v>10</v>
@@ -2733,26 +2733,26 @@
     </row>
     <row r="34" spans="3:13" ht="86.4" x14ac:dyDescent="0.3">
       <c r="C34" s="5" t="s">
-        <v>89</v>
+        <v>76</v>
       </c>
       <c r="D34" s="5" t="s">
-        <v>49</v>
+        <v>39</v>
       </c>
       <c r="E34" s="5"/>
       <c r="F34" s="5" t="s">
-        <v>51</v>
+        <v>109</v>
       </c>
       <c r="G34" s="5" t="s">
         <v>9</v>
       </c>
       <c r="H34" s="5" t="s">
-        <v>103</v>
+        <v>85</v>
       </c>
       <c r="I34" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="J34" s="5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="K34" s="5" t="s">
         <v>10</v>
@@ -2762,28 +2762,28 @@
     </row>
     <row r="35" spans="3:13" ht="230.4" x14ac:dyDescent="0.3">
       <c r="C35" s="3" t="s">
-        <v>110</v>
+        <v>91</v>
       </c>
       <c r="D35" s="5" t="s">
-        <v>56</v>
+        <v>44</v>
       </c>
       <c r="E35" s="5" t="s">
-        <v>57</v>
+        <v>45</v>
       </c>
       <c r="F35" s="5" t="s">
-        <v>60</v>
+        <v>48</v>
       </c>
       <c r="G35" s="5" t="s">
         <v>9</v>
       </c>
       <c r="H35" s="5" t="s">
-        <v>103</v>
+        <v>85</v>
       </c>
       <c r="I35" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="J35" s="5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="K35" s="5" t="s">
         <v>10</v>

</xml_diff>